<commit_message>
added user input and result text
</commit_message>
<xml_diff>
--- a/erice/Erice2.xlsx
+++ b/erice/Erice2.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="77">
   <si>
     <t>Diabetics</t>
   </si>
   <si>
     <t>Non diabetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Non smokers</t>
@@ -1376,7 +1379,7 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="L1:S1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1422,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q1" s="22" t="s">
         <v>1</v>
@@ -1441,49 +1444,49 @@
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="P2" s="23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S2" s="25"/>
     </row>
@@ -1493,7 +1496,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="11">
         <v>5.2</v>
@@ -1553,52 +1556,52 @@
         <v>180</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>7</v>
-      </c>
       <c r="Q4" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S4" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:19">
@@ -1610,52 +1613,52 @@
         <v>160</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>19</v>
-      </c>
       <c r="R5" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1663,58 +1666,58 @@
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="14">
         <v>140</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="14" t="s">
-        <v>12</v>
-      </c>
       <c r="S6" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:19">
@@ -1726,52 +1729,52 @@
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>14</v>
-      </c>
       <c r="Q7" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1783,52 +1786,52 @@
         <v>180</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>38</v>
-      </c>
       <c r="Q8" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="S8" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:19">
@@ -1836,58 +1839,58 @@
         <v>0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14">
         <v>160</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>47</v>
-      </c>
       <c r="G9" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="S9" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="S9" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1899,52 +1902,52 @@
         <v>140</v>
       </c>
       <c r="D10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:19">
@@ -1956,52 +1959,52 @@
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P11" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="S11" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2013,52 +2016,52 @@
         <v>180</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>48</v>
-      </c>
       <c r="L12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="P12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="R12" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:19">
@@ -2070,52 +2073,52 @@
         <v>160</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="9" t="s">
+      <c r="Q13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="P13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="R13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="S13" s="15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2123,58 +2126,58 @@
         <v>0</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="14">
         <v>140</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="1:19">
@@ -2186,52 +2189,52 @@
         <v>0</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="P15" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="Q15" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="S15" s="15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2243,52 +2246,52 @@
         <v>180</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="P16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="L16" s="9" t="s">
+      <c r="Q16" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="S16" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="R16" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="S16" s="15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="1:19">
@@ -2300,52 +2303,52 @@
         <v>160</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q17" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -2353,58 +2356,58 @@
         <v>0</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="14">
         <v>140</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K18" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="L18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P18" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L18" s="9" t="s">
+      <c r="Q18" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="R18" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S18" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="P18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="R18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="S18" s="15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="1:19">
@@ -2416,52 +2419,52 @@
         <v>0</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>63</v>
-      </c>
       <c r="L19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="R19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="P19" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q19" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="R19" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="S19" s="15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -2473,52 +2476,52 @@
         <v>180</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F20" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="I20" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>69</v>
-      </c>
       <c r="J20" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q20" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S20" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" ht="15.75" spans="1:19">
@@ -2530,52 +2533,52 @@
         <v>160</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R21" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -2583,58 +2586,58 @@
         <v>0</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" s="14">
         <v>140</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="I22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="J22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>69</v>
-      </c>
       <c r="K22" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P22" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q22" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="1:19">
@@ -2646,107 +2649,107 @@
         <v>0</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O23" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S23" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:19">
       <c r="A24" s="18"/>
       <c r="B24" s="16"/>
       <c r="C24" s="20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E24" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="I24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="J24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="I24" s="21" t="s">
+      <c r="K24" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="L24" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="M24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="K24" s="24" t="s">
+      <c r="N24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L24" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="M24" s="21" t="s">
+      <c r="O24" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="P24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="N24" s="21" t="s">
+      <c r="Q24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="O24" s="21" t="s">
+      <c r="R24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="P24" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q24" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="R24" s="21" t="s">
-        <v>74</v>
-      </c>
       <c r="S24" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified for age below 49
</commit_message>
<xml_diff>
--- a/erice/Erice2.xlsx
+++ b/erice/Erice2.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="76">
   <si>
     <t>Diabetics</t>
   </si>
   <si>
     <t>Non diabetics</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Non smokers</t>
@@ -1030,7 +1027,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1056,7 +1053,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1379,12 +1375,12 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="R2" sqref="R2:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:19">
+    <row r="1" spans="1:19">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1425,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q1" s="22" t="s">
         <v>1</v>
@@ -1437,58 +1433,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:19">
+    <row r="2" spans="1:19">
       <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>4</v>
-      </c>
       <c r="L2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="Q2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="R2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="S2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="25"/>
     </row>
     <row r="3" ht="15.75" spans="1:19">
       <c r="A3" s="9">
@@ -1496,7 +1494,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="11">
         <v>5.2</v>
@@ -1556,52 +1554,52 @@
         <v>180</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="14" t="s">
+      <c r="K4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="N4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="O4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="14" t="s">
+      <c r="S4" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="S4" s="15" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:19">
@@ -1613,52 +1611,52 @@
         <v>160</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="9" t="s">
+      <c r="R5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="S5" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1666,58 +1664,58 @@
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="14">
         <v>140</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="J6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="15" t="s">
+      <c r="M6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="15" t="s">
+      <c r="O6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="R6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:19">
@@ -1729,52 +1727,52 @@
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="K7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="15" t="s">
+      <c r="O7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="14" t="s">
+      <c r="S7" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="S7" s="15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1786,52 +1784,52 @@
         <v>180</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="G8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="9" t="s">
+      <c r="Q8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="R8" s="14" t="s">
+      <c r="S8" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="S8" s="15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:19">
@@ -1839,58 +1837,58 @@
         <v>0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="14">
         <v>160</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="N9" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="P9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="S9" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1902,52 +1900,52 @@
         <v>140</v>
       </c>
       <c r="D10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="M10" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>56</v>
-      </c>
       <c r="N10" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S10" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:19">
@@ -1959,52 +1957,52 @@
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="14" t="s">
+      <c r="K11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="15" t="s">
-        <v>47</v>
-      </c>
       <c r="L11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11" s="15" t="s">
+      <c r="Q11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="P11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="R11" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="S11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2016,52 +2014,52 @@
         <v>180</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="M12" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="N12" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" s="15" t="s">
+      <c r="O12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="P12" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="Q12" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:19">
@@ -2073,52 +2071,52 @@
         <v>160</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="G13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P13" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="Q13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="S13" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="P13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="R13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="S13" s="15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2126,58 +2124,58 @@
         <v>0</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="14">
         <v>140</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>57</v>
-      </c>
       <c r="L14" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" ht="15.75" spans="1:19">
@@ -2189,52 +2187,52 @@
         <v>0</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="H15" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="S15" s="15" t="s">
         <v>60</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="P15" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q15" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="R15" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="S15" s="15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2246,52 +2244,52 @@
         <v>180</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="H16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="S16" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="R16" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="S16" s="15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="1:19">
@@ -2303,52 +2301,52 @@
         <v>160</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="M17" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q17" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -2356,58 +2354,58 @@
         <v>0</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="14">
         <v>140</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="H18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="15" t="s">
+      <c r="L18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="P18" s="14" t="s">
-        <v>65</v>
-      </c>
       <c r="Q18" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S18" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="1:19">
@@ -2419,52 +2417,52 @@
         <v>0</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q19" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="R19" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="P19" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q19" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="R19" s="14" t="s">
-        <v>66</v>
-      </c>
       <c r="S19" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -2476,52 +2474,52 @@
         <v>180</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q20" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S20" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" ht="15.75" spans="1:19">
@@ -2533,52 +2531,52 @@
         <v>160</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="N21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="P21" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q21" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R21" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -2586,58 +2584,58 @@
         <v>0</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="14">
         <v>140</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P22" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q22" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="1:19">
@@ -2649,107 +2647,107 @@
         <v>0</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S23" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" ht="15.75" spans="1:19">
       <c r="A24" s="18"/>
       <c r="B24" s="16"/>
       <c r="C24" s="20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="F24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="G24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="H24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="J24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="K24" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="K24" s="24" t="s">
-        <v>76</v>
-      </c>
       <c r="L24" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="M24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="M24" s="21" t="s">
+      <c r="N24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N24" s="21" t="s">
+      <c r="O24" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="O24" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="P24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="Q24" s="21" t="s">
+      <c r="R24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="R24" s="21" t="s">
+      <c r="S24" s="24" t="s">
         <v>75</v>
-      </c>
-      <c r="S24" s="24" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>